<commit_message>
ASK-41 fixed almost all problems except combined sections an INNW STPH values.
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmarktest_traject 16-5.xlsx
+++ b/benchmarktests/testdefinitions/Benchmarktest_traject 16-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F892E6B-BCDE-4A30-B91D-46531AF87B87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1887AEA3-BC34-410E-BA2B-E9FBBC7B327D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="8" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="3510" yWindow="525" windowWidth="28800" windowHeight="15435" tabRatio="653" firstSheet="1" activeTab="8" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -2090,18 +2090,18 @@
       <c r="B12" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="31" t="str">
+      <c r="C12" s="31">
         <f>HTKW!C5</f>
-        <v>GR</v>
+        <v>2.8437656524269217E-2</v>
       </c>
       <c r="D12" s="26">
         <f>HTKW!C6</f>
         <v>2.8437656524269217E-2</v>
       </c>
       <c r="E12" s="49"/>
-      <c r="G12" s="1" t="e">
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0.97156234347573078</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="K5" s="9" t="str">
         <f t="array" ref="K5">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B5,C5),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="L5" s="12" t="str">
         <f t="array" ref="L5">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B5,C5),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="K10" s="9" t="str">
         <f t="array" ref="K10">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B10,C10),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="L10" s="12" t="str">
         <f t="array" ref="L10">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B10,C10),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
@@ -3146,7 +3146,7 @@
   <dimension ref="B2:Y32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8902,7 +8902,7 @@
   <dimension ref="B2:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K22"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8926,7 +8926,7 @@
         <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
@@ -9063,15 +9063,15 @@
         <v>NR</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11:M22" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N22" si="3">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11" si="3">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11:O22" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -9079,16 +9079,16 @@
         <v>0</v>
       </c>
       <c r="Q11" s="9">
-        <f t="array" ref="Q11">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J11,'Normen en duidingsklassen'!$E$13:$E$20))</f>
-        <v>0.1</v>
+        <f t="array" ref="Q11">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J11,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <v>0</v>
       </c>
       <c r="R11" s="9">
-        <f>IFERROR(MATCH($Q11,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
-        <v>5</v>
+        <f>IFERROR(MATCH($Q11,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
+        <v>1</v>
       </c>
       <c r="S11" s="9" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,R11)</f>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="T11" s="12" t="b">
         <f>IF($E11="Ja",IF($H11="Ja",NOT(ISNUMBER($I11)),FALSE),FALSE)</f>
@@ -9125,35 +9125,35 @@
         <v>ND</v>
       </c>
       <c r="M12" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M12:M22" si="5">IF(AND(F12="Geen faalkans",H12="Nee"),1,1-J12)</f>
         <v>1</v>
       </c>
       <c r="N12" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="N12:N22" si="6">IF(J12="-",1,M12)</f>
         <v>1</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="O12:O22" si="7">IF(AND(F12="Geen faalkans",H12="Nee"),0,J12*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P22" si="5">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P22" si="8">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
-        <f t="array" ref="Q12">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J12,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <f t="array" ref="Q12">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J12,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>0</v>
       </c>
       <c r="R12" s="9">
-        <f>IFERROR(MATCH($Q12,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
-        <v>4</v>
+        <f>IFERROR(MATCH($Q12,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
+        <v>1</v>
       </c>
       <c r="S12" s="9" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,R12)</f>
-        <v>+0</v>
+        <v>+III</v>
       </c>
       <c r="T12" s="12" t="b">
-        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="9">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -9188,38 +9188,38 @@
       </c>
       <c r="K13" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q13" s="9">
-        <f t="array" ref="Q13">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J13,'Normen en duidingsklassen'!$E$13:$E$20))</f>
-        <v>0.1</v>
+        <f t="array" ref="Q13">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J13,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <v>0</v>
       </c>
       <c r="R13" s="9">
-        <f>IFERROR(MATCH($Q13,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
-        <v>5</v>
+        <f>IFERROR(MATCH($Q13,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
+        <v>1</v>
       </c>
       <c r="S13" s="9" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,R13)</f>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="T13" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9255,27 +9255,27 @@
         <v>-I</v>
       </c>
       <c r="M14" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.99977199999999999</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99977199999999999</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="Q14" s="9">
-        <f t="array" ref="Q14">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J14,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <f t="array" ref="Q14">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J14,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>0.1</v>
       </c>
       <c r="R14" s="9">
-        <f>IFERROR(MATCH($Q14,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
+        <f>IFERROR(MATCH($Q14,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
         <v>5</v>
       </c>
       <c r="S14" s="9" t="str">
@@ -9283,7 +9283,7 @@
         <v>-I</v>
       </c>
       <c r="T14" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9321,27 +9321,27 @@
         <v>-I</v>
       </c>
       <c r="M15" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.99673</v>
       </c>
       <c r="N15" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99673</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="Q15" s="9">
-        <f t="array" ref="Q15">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J15,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <f t="array" ref="Q15">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J15,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>0.1</v>
       </c>
       <c r="R15" s="9">
-        <f>IFERROR(MATCH($Q15,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
+        <f>IFERROR(MATCH($Q15,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
         <v>5</v>
       </c>
       <c r="S15" s="9" t="str">
@@ -9349,7 +9349,7 @@
         <v>-I</v>
       </c>
       <c r="T15" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9383,35 +9383,35 @@
         <v>NR</v>
       </c>
       <c r="M16" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
-        <f t="array" ref="Q16">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J16,'Normen en duidingsklassen'!$E$13:$E$20))</f>
-        <v>0.1</v>
+        <f t="array" ref="Q16">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J16,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <v>0</v>
       </c>
       <c r="R16" s="9">
-        <f>IFERROR(MATCH($Q16,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
-        <v>5</v>
+        <f>IFERROR(MATCH($Q16,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
+        <v>1</v>
       </c>
       <c r="S16" s="9" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,R16)</f>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="T16" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9445,35 +9445,35 @@
         <v>NR</v>
       </c>
       <c r="M17" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q17" s="9">
-        <f t="array" ref="Q17">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J17,'Normen en duidingsklassen'!$E$13:$E$20))</f>
-        <v>0.1</v>
+        <f t="array" ref="Q17">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J17,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <v>0</v>
       </c>
       <c r="R17" s="9">
-        <f>IFERROR(MATCH($Q17,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
-        <v>5</v>
+        <f>IFERROR(MATCH($Q17,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
+        <v>1</v>
       </c>
       <c r="S17" s="9" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,R17)</f>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="T17" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9506,38 +9506,38 @@
       </c>
       <c r="K18" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="M18" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q18" s="9">
-        <f t="array" ref="Q18">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J18,'Normen en duidingsklassen'!$E$13:$E$20))</f>
-        <v>0.1</v>
+        <f t="array" ref="Q18">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J18,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <v>0</v>
       </c>
       <c r="R18" s="9">
-        <f>IFERROR(MATCH($Q18,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
-        <v>5</v>
+        <f>IFERROR(MATCH($Q18,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
+        <v>1</v>
       </c>
       <c r="S18" s="9" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,R18)</f>
-        <v>-I</v>
+        <v>+III</v>
       </c>
       <c r="T18" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9573,35 +9573,35 @@
         <v>D</v>
       </c>
       <c r="M19" s="31" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O19" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q19" s="9">
-        <f t="array" ref="Q19">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J19,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <f t="array" ref="Q19">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J19,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>0</v>
       </c>
       <c r="R19" s="9">
-        <f>IFERROR(MATCH($Q19,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
-        <v>4</v>
+        <f>IFERROR(MATCH($Q19,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
+        <v>1</v>
       </c>
       <c r="S19" s="9" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,R19)</f>
-        <v>+0</v>
+        <v>+III</v>
       </c>
       <c r="T19" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -9629,7 +9629,7 @@
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="10">
-        <f t="shared" ref="J20:J22" si="7">IF($E20="Nee",0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
+        <f t="shared" ref="J20:J22" si="10">IF($E20="Nee",0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-")))</f>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="K20" s="32" t="str">
@@ -9637,27 +9637,27 @@
         <v>-I</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.99999800000000005</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99999800000000005</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="Q20" s="9">
-        <f t="array" ref="Q20">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J20,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <f t="array" ref="Q20">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J20,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>0.1</v>
       </c>
       <c r="R20" s="9">
-        <f>IFERROR(MATCH($Q20,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
+        <f>IFERROR(MATCH($Q20,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
         <v>5</v>
       </c>
       <c r="S20" s="9" t="str">
@@ -9665,7 +9665,7 @@
         <v>-I</v>
       </c>
       <c r="T20" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9695,7 +9695,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K21" s="32" t="str">
@@ -9703,27 +9703,27 @@
         <v>-I</v>
       </c>
       <c r="M21" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.99950000000000006</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99950000000000006</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q21" s="9">
-        <f t="array" ref="Q21">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J21,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <f t="array" ref="Q21">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J21,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>0.1</v>
       </c>
       <c r="R21" s="9">
-        <f>IFERROR(MATCH($Q21,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
+        <f>IFERROR(MATCH($Q21,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
         <v>5</v>
       </c>
       <c r="S21" s="9" t="str">
@@ -9731,7 +9731,7 @@
         <v>-I</v>
       </c>
       <c r="T21" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -9759,7 +9759,7 @@
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="K22" s="32" t="str">
@@ -9767,27 +9767,27 @@
         <v>-I</v>
       </c>
       <c r="M22" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.99999999799999995</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99999999799999995</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="Q22" s="9">
-        <f t="array" ref="Q22">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;$J22,'Normen en duidingsklassen'!$E$13:$E$20))</f>
+        <f t="array" ref="Q22">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$J22,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>0.1</v>
       </c>
       <c r="R22" s="9">
-        <f>IFERROR(MATCH($Q22,'Normen en duidingsklassen'!$E$13:$E$20),1)</f>
+        <f>IFERROR(MATCH($Q22,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
         <v>5</v>
       </c>
       <c r="S22" s="9" t="str">
@@ -9795,7 +9795,7 @@
         <v>-I</v>
       </c>
       <c r="T22" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -10042,7 +10042,7 @@
   <dimension ref="B2:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10089,9 +10089,9 @@
       <c r="B5" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="26" t="str">
+      <c r="C5" s="26">
         <f>IFERROR(MIN(1-PRODUCT(M11:M27),MAX(O11:O27)),"GR")</f>
-        <v>GR</v>
+        <v>2.8437656524269217E-2</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
@@ -10187,7 +10187,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="3" t="s">
@@ -10202,17 +10202,17 @@
         <f t="shared" ref="K11:K22" si="1">IF($E11="Nee","NR",IF(ISNUMBER($J11),S11,IF($T11,"D","ND")))</f>
         <v>ND</v>
       </c>
-      <c r="M11" s="31" t="e">
+      <c r="M11" s="31">
         <f t="shared" ref="M11:M12" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="N11" s="10">
         <f t="shared" ref="N11:N12" si="3">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
-      <c r="O11" s="10" t="e">
+      <c r="O11" s="10">
         <f>IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="P11" s="10">
         <f>IF(J11="-",0,O11)</f>
@@ -11148,7 +11148,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{66D3252B-4C33-455B-8361-35393CCA4B04}">
           <x14:formula1>
             <xm:f>Informatiepagina!$B$15:$B$17</xm:f>

</xml_diff>

<commit_message>
ASK-68 Let TranslateAssessentResultAggregatedMethod return a probability of0.0 in ase of NotDominant and adjust expectations accordingly
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmarktest_traject 16-5.xlsx
+++ b/benchmarktests/testdefinitions/Benchmarktest_traject 16-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504942E0-A7B6-431F-93AB-1037C892B012}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D684CAE1-2667-42A1-8E57-11A4814BC60E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="653" firstSheet="1" activeTab="2" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="653" firstSheet="1" activeTab="3" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -741,72 +741,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="0"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="0"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="82">
     <dxf>
       <fill>
         <patternFill>
@@ -3221,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49710E67-B736-4749-B620-06835F5DE469}">
   <dimension ref="B2:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,19 +3333,19 @@
       <c r="J11" s="5"/>
       <c r="K11" s="25"/>
       <c r="L11" s="29">
-        <f>IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF($X11=TRUE,IF(ISNUMBER($J11),J11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
+        <f>IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF($I11="Ja",IF(ISNUMBER(J11),J11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
         <v>0</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" ref="M11:M22" si="0">IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF(I11="Ja",IF(ISNUMBER(K11),K11,"-"),IF(ISNUMBER(H11),H11,"-"))))</f>
+        <f>IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF($I11="Ja",IF(ISNUMBER(K11),K11,"-"),IF(ISNUMBER(H11),H11,"-"))))</f>
         <v>0</v>
       </c>
       <c r="N11" s="6">
-        <f t="shared" ref="N11:N22" si="1">IF(ISNUMBER(L11),IF(M11=0,1,M11/L11),"-")</f>
+        <f t="shared" ref="N11:N22" si="0">IF(ISNUMBER(L11),IF(M11=0,1,M11/L11),"-")</f>
         <v>1</v>
       </c>
       <c r="O11" s="30" t="str">
-        <f>IF($Z11=TRUE,"NR",IF($Y11=TRUE,"ND",IF($X11=TRUE,"D",W11)))</f>
+        <f t="shared" ref="O11:O22" si="1">IF($Z11=TRUE,"NR",IF($Y11=TRUE,"ND",IF($X11=TRUE,"D",W11)))</f>
         <v>ND</v>
       </c>
       <c r="Q11" s="31">
@@ -3483,19 +3418,19 @@
       <c r="J12" s="10"/>
       <c r="K12" s="26"/>
       <c r="L12" s="31">
-        <f>IF($Z12=TRUE,0,IF($Y12=TRUE,0,IF($X12=TRUE,IF(ISNUMBER($J12),J12,"-"),IF(ISNUMBER(G12),G12,"-"))))</f>
+        <f t="shared" ref="L12:L22" si="5">IF($Z12=TRUE,0,IF($Y12=TRUE,0,IF($I12="Ja",IF(ISNUMBER(J12),J12,"-"),IF(ISNUMBER(G12),G12,"-"))))</f>
         <v>0</v>
       </c>
       <c r="M12" s="10">
+        <f t="shared" ref="M12:M22" si="6">IF($Z12=TRUE,0,IF($Y12=TRUE,0,IF($I12="Ja",IF(ISNUMBER(K12),K12,"-"),IF(ISNUMBER(H12),H12,"-"))))</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="11">
+        <v>1</v>
+      </c>
+      <c r="O12" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="32" t="str">
-        <f>IF($Z12=TRUE,"NR",IF($Y12=TRUE,"ND",IF($X12=TRUE,"D",W12)))</f>
         <v>+III</v>
       </c>
       <c r="Q12" s="31">
@@ -3503,7 +3438,7 @@
         <v>1</v>
       </c>
       <c r="R12" s="10">
-        <f t="shared" ref="R12:R22" si="5">IF(M12="-",1,Q12)</f>
+        <f t="shared" ref="R12:R22" si="7">IF(M12="-",1,Q12)</f>
         <v>1</v>
       </c>
       <c r="S12" s="10">
@@ -3511,7 +3446,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="10">
-        <f t="shared" ref="T12:T22" si="6">IF(L12="-",0,S12)</f>
+        <f t="shared" ref="T12:T22" si="8">IF(L12="-",0,S12)</f>
         <v>0</v>
       </c>
       <c r="U12" s="9">
@@ -3527,15 +3462,15 @@
         <v>+III</v>
       </c>
       <c r="X12" s="9" t="b">
-        <f t="shared" ref="X12:X22" si="7">IF($E12="Ja",IF($I12="Ja",NOT(ISNUMBER($J12)),FALSE),FALSE)</f>
+        <f t="shared" ref="X12:X22" si="9">IF($E12="Ja",IF($I12="Ja",NOT(ISNUMBER($J12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Y12" s="9" t="b">
-        <f t="shared" ref="Y12:Y22" si="8">IF($E12="Ja",IF($I12="Nee",OR(NOT(ISNUMBER($G12)),NOT(ISNUMBER($H12))),FALSE),FALSE)</f>
+        <f t="shared" ref="Y12:Y22" si="10">IF($E12="Ja",IF($I12="Nee",OR(NOT(ISNUMBER($G12)),NOT(ISNUMBER($H12))),FALSE),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z12" s="12" t="b">
-        <f t="shared" ref="Z12:Z22" si="9">IF($E12="Nee",TRUE,FALSE)</f>
+        <f t="shared" ref="Z12:Z22" si="11">IF($E12="Nee",TRUE,FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -3571,19 +3506,19 @@
         <v>0</v>
       </c>
       <c r="L13" s="31">
-        <f>IF($Z13=TRUE,0,IF($Y13=TRUE,0,IF($X13=TRUE,IF(ISNUMBER($J13),J13,"-"),IF(ISNUMBER(G13),G13,"-"))))</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="M13" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="11">
+        <v>1</v>
+      </c>
+      <c r="O13" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O13" s="32" t="str">
-        <f>IF($Z13=TRUE,"NR",IF($Y13=TRUE,"ND",IF($X13=TRUE,"D",W13)))</f>
         <v>+III</v>
       </c>
       <c r="Q13" s="31">
@@ -3591,16 +3526,16 @@
         <v>1</v>
       </c>
       <c r="R13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S13" s="10">
         <f t="shared" si="3"/>
-        <v>28.9</v>
+        <v>0</v>
       </c>
       <c r="T13" s="10">
-        <f t="shared" si="6"/>
-        <v>28.9</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="U13" s="9">
         <f t="array" ref="U13">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M13,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -3615,15 +3550,15 @@
         <v>+III</v>
       </c>
       <c r="X13" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y13" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z13" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3656,19 +3591,19 @@
       <c r="J14" s="10"/>
       <c r="K14" s="26"/>
       <c r="L14" s="31" t="str">
-        <f>IF($Z14=TRUE,0,IF($Y14=TRUE,0,IF($X14=TRUE,IF(ISNUMBER($J14),J14,"-"),IF(ISNUMBER(G14),G14,"-"))))</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M14" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="N14" s="11" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="N14" s="11" t="str">
+      <c r="O14" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="O14" s="32" t="str">
-        <f>IF($Z14=TRUE,"NR",IF($Y14=TRUE,"ND",IF($X14=TRUE,"D",W14)))</f>
         <v>D</v>
       </c>
       <c r="Q14" s="31" t="e">
@@ -3676,7 +3611,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="R14" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S14" s="10" t="e">
@@ -3684,7 +3619,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="T14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U14" s="9">
@@ -3700,15 +3635,15 @@
         <v>+III</v>
       </c>
       <c r="X14" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Y14" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z14" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3744,19 +3679,19 @@
         <v>1.8300000000000001E-5</v>
       </c>
       <c r="L15" s="31">
-        <f>IF($Z15=TRUE,0,IF($Y15=TRUE,0,IF($X15=TRUE,IF(ISNUMBER($J15),J15,"-"),IF(ISNUMBER(G15),G15,"-"))))</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="M15" s="10">
+        <f t="shared" si="6"/>
+        <v>1.8300000000000001E-5</v>
+      </c>
+      <c r="N15" s="11">
         <f t="shared" si="0"/>
-        <v>1.8300000000000001E-5</v>
-      </c>
-      <c r="N15" s="11">
+        <v>3.6599999999999997</v>
+      </c>
+      <c r="O15" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>1.8300000000000001E-5</v>
-      </c>
-      <c r="O15" s="32" t="str">
-        <f>IF($Z15=TRUE,"NR",IF($Y15=TRUE,"ND",IF($X15=TRUE,"D",W15)))</f>
         <v>-I</v>
       </c>
       <c r="Q15" s="31">
@@ -3764,16 +3699,16 @@
         <v>0.99998169999999997</v>
       </c>
       <c r="R15" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99998169999999997</v>
       </c>
       <c r="S15" s="10">
         <f t="shared" si="3"/>
-        <v>28.9</v>
+        <v>1.4450000000000002E-4</v>
       </c>
       <c r="T15" s="10">
-        <f t="shared" si="6"/>
-        <v>28.9</v>
+        <f t="shared" si="8"/>
+        <v>1.4450000000000002E-4</v>
       </c>
       <c r="U15" s="9">
         <f t="array" ref="U15">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M15,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -3788,15 +3723,15 @@
         <v>-I</v>
       </c>
       <c r="X15" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y15" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z15" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3824,19 +3759,19 @@
       <c r="J16" s="10"/>
       <c r="K16" s="26"/>
       <c r="L16" s="31">
-        <f>IF($Z16=TRUE,0,IF($Y16=TRUE,0,IF($X16=TRUE,IF(ISNUMBER($J16),J16,"-"),IF(ISNUMBER(G16),G16,"-"))))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M16" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="11">
+        <v>1</v>
+      </c>
+      <c r="O16" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="32" t="str">
-        <f>IF($Z16=TRUE,"NR",IF($Y16=TRUE,"ND",IF($X16=TRUE,"D",W16)))</f>
         <v>NR</v>
       </c>
       <c r="Q16" s="31">
@@ -3844,7 +3779,7 @@
         <v>1</v>
       </c>
       <c r="R16" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S16" s="10">
@@ -3852,7 +3787,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U16" s="9">
@@ -3868,15 +3803,15 @@
         <v>+III</v>
       </c>
       <c r="X16" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y16" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z16" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -3904,19 +3839,19 @@
       <c r="J17" s="10"/>
       <c r="K17" s="26"/>
       <c r="L17" s="31">
-        <f>IF($Z17=TRUE,0,IF($Y17=TRUE,0,IF($X17=TRUE,IF(ISNUMBER($J17),J17,"-"),IF(ISNUMBER(G17),G17,"-"))))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M17" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="11">
+        <v>1</v>
+      </c>
+      <c r="O17" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O17" s="32" t="str">
-        <f>IF($Z17=TRUE,"NR",IF($Y17=TRUE,"ND",IF($X17=TRUE,"D",W17)))</f>
         <v>NR</v>
       </c>
       <c r="Q17" s="31">
@@ -3924,7 +3859,7 @@
         <v>1</v>
       </c>
       <c r="R17" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S17" s="10">
@@ -3932,7 +3867,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U17" s="9">
@@ -3948,15 +3883,15 @@
         <v>+III</v>
       </c>
       <c r="X17" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y17" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z17" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -3984,19 +3919,19 @@
       <c r="J18" s="10"/>
       <c r="K18" s="26"/>
       <c r="L18" s="31">
-        <f>IF($Z18=TRUE,0,IF($Y18=TRUE,0,IF($X18=TRUE,IF(ISNUMBER($J18),J18,"-"),IF(ISNUMBER(G18),G18,"-"))))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M18" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="11">
+        <v>1</v>
+      </c>
+      <c r="O18" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O18" s="32" t="str">
-        <f>IF($Z18=TRUE,"NR",IF($Y18=TRUE,"ND",IF($X18=TRUE,"D",W18)))</f>
         <v>NR</v>
       </c>
       <c r="Q18" s="31">
@@ -4004,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="R18" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S18" s="10">
@@ -4012,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U18" s="9">
@@ -4028,15 +3963,15 @@
         <v>+III</v>
       </c>
       <c r="X18" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y18" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z18" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -4060,7 +3995,7 @@
         <v>7.27E-4</v>
       </c>
       <c r="H19" s="26">
-        <f t="shared" ref="H19:H22" si="10">G19*3.66</f>
+        <f t="shared" ref="H19:H22" si="12">G19*3.66</f>
         <v>2.6608199999999999E-3</v>
       </c>
       <c r="I19" s="8" t="s">
@@ -4069,19 +4004,19 @@
       <c r="J19" s="10"/>
       <c r="K19" s="26"/>
       <c r="L19" s="31">
-        <f>IF($Z19=TRUE,0,IF($Y19=TRUE,0,IF($X19=TRUE,IF(ISNUMBER($J19),J19,"-"),IF(ISNUMBER(G19),G19,"-"))))</f>
+        <f t="shared" si="5"/>
         <v>7.27E-4</v>
       </c>
       <c r="M19" s="10">
+        <f t="shared" si="6"/>
+        <v>2.6608199999999999E-3</v>
+      </c>
+      <c r="N19" s="11">
         <f t="shared" si="0"/>
-        <v>2.6608199999999999E-3</v>
-      </c>
-      <c r="N19" s="11">
+        <v>3.66</v>
+      </c>
+      <c r="O19" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>3.66</v>
-      </c>
-      <c r="O19" s="32" t="str">
-        <f>IF($Z19=TRUE,"NR",IF($Y19=TRUE,"ND",IF($X19=TRUE,"D",W19)))</f>
         <v>-I</v>
       </c>
       <c r="Q19" s="31">
@@ -4089,7 +4024,7 @@
         <v>0.99733917999999999</v>
       </c>
       <c r="R19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99733917999999999</v>
       </c>
       <c r="S19" s="10">
@@ -4097,7 +4032,7 @@
         <v>2.1010299999999999E-2</v>
       </c>
       <c r="T19" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.1010299999999999E-2</v>
       </c>
       <c r="U19" s="9">
@@ -4113,15 +4048,15 @@
         <v>-I</v>
       </c>
       <c r="X19" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y19" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z19" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4145,7 +4080,7 @@
         <v>7.2800000000000002E-4</v>
       </c>
       <c r="H20" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.6644800000000003E-3</v>
       </c>
       <c r="I20" s="8" t="s">
@@ -4158,19 +4093,19 @@
         <v>0</v>
       </c>
       <c r="L20" s="31">
-        <f>IF($Z20=TRUE,0,IF($Y20=TRUE,0,IF($X20=TRUE,IF(ISNUMBER($J20),J20,"-"),IF(ISNUMBER(G20),G20,"-"))))</f>
-        <v>7.2800000000000002E-4</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="M20" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="11">
+        <v>1</v>
+      </c>
+      <c r="O20" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="32" t="str">
-        <f>IF($Z20=TRUE,"NR",IF($Y20=TRUE,"ND",IF($X20=TRUE,"D",W20)))</f>
         <v>+III</v>
       </c>
       <c r="Q20" s="31">
@@ -4178,16 +4113,16 @@
         <v>1</v>
       </c>
       <c r="R20" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S20" s="10">
         <f t="shared" si="3"/>
-        <v>2.1039200000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="6"/>
-        <v>2.1039200000000001E-2</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="U20" s="9">
         <f t="array" ref="U20">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M20,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -4202,15 +4137,15 @@
         <v>+III</v>
       </c>
       <c r="X20" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y20" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z20" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4234,7 +4169,7 @@
         <v>1E-10</v>
       </c>
       <c r="H21" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.6600000000000003E-10</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -4243,19 +4178,19 @@
       <c r="J21" s="10"/>
       <c r="K21" s="26"/>
       <c r="L21" s="31">
-        <f>IF($Z21=TRUE,0,IF($Y21=TRUE,0,IF($X21=TRUE,IF(ISNUMBER($J21),J21,"-"),IF(ISNUMBER(G21),G21,"-"))))</f>
+        <f t="shared" si="5"/>
         <v>1E-10</v>
       </c>
       <c r="M21" s="10">
+        <f t="shared" si="6"/>
+        <v>3.6600000000000003E-10</v>
+      </c>
+      <c r="N21" s="11">
         <f t="shared" si="0"/>
-        <v>3.6600000000000003E-10</v>
-      </c>
-      <c r="N21" s="11">
+        <v>3.66</v>
+      </c>
+      <c r="O21" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>3.66</v>
-      </c>
-      <c r="O21" s="32" t="str">
-        <f>IF($Z21=TRUE,"NR",IF($Y21=TRUE,"ND",IF($X21=TRUE,"D",W21)))</f>
         <v>-I</v>
       </c>
       <c r="Q21" s="31">
@@ -4263,7 +4198,7 @@
         <v>0.99999999963399999</v>
       </c>
       <c r="R21" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99999999963399999</v>
       </c>
       <c r="S21" s="10">
@@ -4271,7 +4206,7 @@
         <v>2.8900000000000002E-9</v>
       </c>
       <c r="T21" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.8900000000000002E-9</v>
       </c>
       <c r="U21" s="9">
@@ -4287,15 +4222,15 @@
         <v>-I</v>
       </c>
       <c r="X21" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y21" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z21" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4319,7 +4254,7 @@
         <v>1E-4</v>
       </c>
       <c r="H22" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.6600000000000001E-4</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -4328,19 +4263,19 @@
       <c r="J22" s="10"/>
       <c r="K22" s="26"/>
       <c r="L22" s="31">
-        <f>IF($Z22=TRUE,0,IF($Y22=TRUE,0,IF($X22=TRUE,IF(ISNUMBER($J22),J22,"-"),IF(ISNUMBER(G22),G22,"-"))))</f>
+        <f t="shared" si="5"/>
         <v>1E-4</v>
       </c>
       <c r="M22" s="10">
+        <f t="shared" si="6"/>
+        <v>3.6600000000000001E-4</v>
+      </c>
+      <c r="N22" s="11">
         <f t="shared" si="0"/>
-        <v>3.6600000000000001E-4</v>
-      </c>
-      <c r="N22" s="11">
+        <v>3.6599999999999997</v>
+      </c>
+      <c r="O22" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>3.6599999999999997</v>
-      </c>
-      <c r="O22" s="32" t="str">
-        <f>IF($Z22=TRUE,"NR",IF($Y22=TRUE,"ND",IF($X22=TRUE,"D",W22)))</f>
         <v>-I</v>
       </c>
       <c r="Q22" s="31">
@@ -4348,7 +4283,7 @@
         <v>0.99963400000000002</v>
       </c>
       <c r="R22" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99963400000000002</v>
       </c>
       <c r="S22" s="10">
@@ -4356,7 +4291,7 @@
         <v>2.8900000000000002E-3</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.8900000000000002E-3</v>
       </c>
       <c r="U22" s="9">
@@ -4372,15 +4307,15 @@
         <v>-I</v>
       </c>
       <c r="X22" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y22" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z22" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4600,23 +4535,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11:H30">
-    <cfRule type="expression" dxfId="90" priority="11">
+    <cfRule type="expression" dxfId="81" priority="11">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:K30">
-    <cfRule type="expression" dxfId="89" priority="10">
+    <cfRule type="expression" dxfId="80" priority="10">
       <formula>IF($I11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11:O30">
-    <cfRule type="cellIs" dxfId="88" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4714,8 +4649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFA30DD-EAF1-4973-B290-E12CB5036732}">
   <dimension ref="B2:Z32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4895,15 +4830,15 @@
       <c r="J11" s="5"/>
       <c r="K11" s="25"/>
       <c r="L11" s="29">
-        <f>IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF($X11=TRUE,IF(ISNUMBER($J11),J11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
+        <f>IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF($I11="Ja",IF(ISNUMBER(J11),J11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
         <v>0</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" ref="M11:M21" si="0">IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF(I11="Ja",IF(ISNUMBER(K11),K11,"-"),IF(ISNUMBER(H11),H11,"-"))))</f>
+        <f>IF($Z11=TRUE,0,IF($Y11=TRUE,0,IF($I11="Ja",IF(ISNUMBER(K11),K11,"-"),IF(ISNUMBER(H11),H11,"-"))))</f>
         <v>0</v>
       </c>
       <c r="N11" s="6">
-        <f t="shared" ref="N11:N22" si="1">IF(ISNUMBER(L11),IF(M11=0,1,M11/L11),"-")</f>
+        <f t="shared" ref="N11:N22" si="0">IF(ISNUMBER(L11),IF(M11=0,1,M11/L11),"-")</f>
         <v>1</v>
       </c>
       <c r="O11" s="30" t="str">
@@ -4911,7 +4846,7 @@
         <v>+III</v>
       </c>
       <c r="Q11" s="31">
-        <f t="shared" ref="Q11:Q22" si="2">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
+        <f t="shared" ref="Q11:Q22" si="1">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
         <v>1</v>
       </c>
       <c r="R11" s="10">
@@ -4919,7 +4854,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="10">
-        <f t="shared" ref="S11:S22" si="3">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
+        <f t="shared" ref="S11:S22" si="2">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="T11" s="10">
@@ -4979,35 +4914,35 @@
       <c r="J12" s="10"/>
       <c r="K12" s="26"/>
       <c r="L12" s="31">
-        <f t="shared" ref="L12:L22" si="4">IF($Z12=TRUE,0,IF($Y12=TRUE,0,IF($X12=TRUE,IF(ISNUMBER($J12),J12,"-"),IF(ISNUMBER(G12),G12,"-"))))</f>
+        <f>IF($Z12=TRUE,0,IF($Y12=TRUE,0,IF($I12="Ja",IF(ISNUMBER(J12),J12,"-"),IF(ISNUMBER(G12),G12,"-"))))</f>
         <v>2.3699999999999999E-4</v>
       </c>
       <c r="M12" s="10">
+        <f>IF($Z12=TRUE,0,IF($Y12=TRUE,0,IF($I12="Ja",IF(ISNUMBER(K12),K12,"-"),IF(ISNUMBER(H12),H12,"-"))))</f>
+        <v>5.4984000000000001E-4</v>
+      </c>
+      <c r="N12" s="11">
         <f t="shared" si="0"/>
-        <v>5.4984000000000001E-4</v>
-      </c>
-      <c r="N12" s="11">
+        <v>2.3200000000000003</v>
+      </c>
+      <c r="O12" s="32" t="str">
+        <f t="shared" ref="O12:O22" si="3">IF($Z12=TRUE,"NR",IF($Y12=TRUE,"ND",IF($X12=TRUE,"D",W12)))</f>
+        <v>-I</v>
+      </c>
+      <c r="Q12" s="31">
         <f t="shared" si="1"/>
-        <v>2.3200000000000003</v>
-      </c>
-      <c r="O12" s="32" t="str">
-        <f t="shared" ref="O12:O22" si="5">IF($Z12=TRUE,"NR",IF($Y12=TRUE,"ND",IF($X12=TRUE,"D",W12)))</f>
-        <v>-I</v>
-      </c>
-      <c r="Q12" s="31">
+        <v>0.99945015999999998</v>
+      </c>
+      <c r="R12" s="10">
+        <f t="shared" ref="R12:R22" si="4">IF(M12="-",1,Q12)</f>
+        <v>0.99945015999999998</v>
+      </c>
+      <c r="S12" s="10">
         <f t="shared" si="2"/>
-        <v>0.99945015999999998</v>
-      </c>
-      <c r="R12" s="10">
-        <f t="shared" ref="R12:R22" si="6">IF(M12="-",1,Q12)</f>
-        <v>0.99945015999999998</v>
-      </c>
-      <c r="S12" s="10">
-        <f t="shared" si="3"/>
         <v>3.5076E-3</v>
       </c>
       <c r="T12" s="10">
-        <f t="shared" ref="T12:T22" si="7">IF(L12="-",0,S12)</f>
+        <f t="shared" ref="T12:T22" si="5">IF(L12="-",0,S12)</f>
         <v>3.5076E-3</v>
       </c>
       <c r="U12" s="9">
@@ -5023,15 +4958,15 @@
         <v>-I</v>
       </c>
       <c r="X12" s="9" t="b">
-        <f t="shared" ref="X12:X22" si="8">IF($E12="Ja",IF($I12="Ja",OR(NOT(ISNUMBER($J12)),NOT(ISNUMBER($K12))),FALSE),FALSE)</f>
+        <f t="shared" ref="X12:X22" si="6">IF($E12="Ja",IF($I12="Ja",OR(NOT(ISNUMBER($J12)),NOT(ISNUMBER($K12))),FALSE),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Y12" s="9" t="b">
-        <f t="shared" ref="Y12:Y22" si="9">IF($E12="Ja",IF($I12="Nee",OR(NOT(ISNUMBER($G12)),NOT(ISNUMBER($H12))),FALSE),FALSE)</f>
+        <f t="shared" ref="Y12:Y22" si="7">IF($E12="Ja",IF($I12="Nee",OR(NOT(ISNUMBER($G12)),NOT(ISNUMBER($H12))),FALSE),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z12" s="12" t="b">
-        <f t="shared" ref="Z12:Z22" si="10">IF($E12="Nee",TRUE,FALSE)</f>
+        <f t="shared" ref="Z12:Z22" si="8">IF($E12="Nee",TRUE,FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -5063,35 +4998,35 @@
       <c r="J13" s="10"/>
       <c r="K13" s="26"/>
       <c r="L13" s="31">
+        <f>IF($Z13=TRUE,0,IF($Y13=TRUE,0,IF($I13="Ja",IF(ISNUMBER(J13),J13,"-"),IF(ISNUMBER(G13),G13,"-"))))</f>
+        <v>1E-50</v>
+      </c>
+      <c r="M13" s="10">
+        <f>IF($Z13=TRUE,0,IF($Y13=TRUE,0,IF($I13="Ja",IF(ISNUMBER(K13),K13,"-"),IF(ISNUMBER(H13),H13,"-"))))</f>
+        <v>2.3200000000000003E-50</v>
+      </c>
+      <c r="N13" s="11">
+        <f t="shared" si="0"/>
+        <v>2.3200000000000003</v>
+      </c>
+      <c r="O13" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>-I</v>
+      </c>
+      <c r="Q13" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R13" s="10">
         <f t="shared" si="4"/>
-        <v>1E-50</v>
-      </c>
-      <c r="M13" s="10">
-        <f t="shared" si="0"/>
-        <v>2.3200000000000003E-50</v>
-      </c>
-      <c r="N13" s="11">
-        <f t="shared" si="1"/>
-        <v>2.3200000000000003</v>
-      </c>
-      <c r="O13" s="32" t="str">
+        <v>1</v>
+      </c>
+      <c r="S13" s="10">
+        <f t="shared" si="2"/>
+        <v>1.48E-49</v>
+      </c>
+      <c r="T13" s="10">
         <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="Q13" s="31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="R13" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S13" s="10">
-        <f t="shared" si="3"/>
-        <v>1.48E-49</v>
-      </c>
-      <c r="T13" s="10">
-        <f t="shared" si="7"/>
         <v>1.48E-49</v>
       </c>
       <c r="U13" s="9">
@@ -5107,15 +5042,15 @@
         <v>-I</v>
       </c>
       <c r="X13" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z13" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5143,35 +5078,35 @@
       <c r="J14" s="10"/>
       <c r="K14" s="26"/>
       <c r="L14" s="31">
+        <f>IF($Z14=TRUE,0,IF($Y14=TRUE,0,IF($I14="Ja",IF(ISNUMBER(J14),J14,"-"),IF(ISNUMBER(G14),G14,"-"))))</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="10">
+        <f>IF($Z14=TRUE,0,IF($Y14=TRUE,0,IF($I14="Ja",IF(ISNUMBER(K14),K14,"-"),IF(ISNUMBER(H14),H14,"-"))))</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>NR</v>
+      </c>
+      <c r="Q14" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R14" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="32" t="str">
+        <v>1</v>
+      </c>
+      <c r="S14" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="10">
         <f t="shared" si="5"/>
-        <v>NR</v>
-      </c>
-      <c r="Q14" s="31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="R14" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S14" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="10">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U14" s="9">
@@ -5187,15 +5122,15 @@
         <v>+III</v>
       </c>
       <c r="X14" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y14" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -5227,35 +5162,35 @@
       <c r="J15" s="10"/>
       <c r="K15" s="26"/>
       <c r="L15" s="31">
+        <f>IF($Z15=TRUE,0,IF($Y15=TRUE,0,IF($I15="Ja",IF(ISNUMBER(J15),J15,"-"),IF(ISNUMBER(G15),G15,"-"))))</f>
+        <v>2.3751999999999999E-4</v>
+      </c>
+      <c r="M15" s="10">
+        <f>IF($Z15=TRUE,0,IF($Y15=TRUE,0,IF($I15="Ja",IF(ISNUMBER(K15),K15,"-"),IF(ISNUMBER(H15),H15,"-"))))</f>
+        <v>5.5104640000000005E-4</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="0"/>
+        <v>2.3200000000000003</v>
+      </c>
+      <c r="O15" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>-I</v>
+      </c>
+      <c r="Q15" s="31">
+        <f t="shared" si="1"/>
+        <v>0.99944895359999997</v>
+      </c>
+      <c r="R15" s="10">
         <f t="shared" si="4"/>
-        <v>2.3751999999999999E-4</v>
-      </c>
-      <c r="M15" s="10">
-        <f t="shared" si="0"/>
-        <v>5.5104640000000005E-4</v>
-      </c>
-      <c r="N15" s="11">
-        <f t="shared" si="1"/>
-        <v>2.3200000000000003</v>
-      </c>
-      <c r="O15" s="32" t="str">
+        <v>0.99944895359999997</v>
+      </c>
+      <c r="S15" s="10">
+        <f t="shared" si="2"/>
+        <v>3.5152960000000002E-3</v>
+      </c>
+      <c r="T15" s="10">
         <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="Q15" s="31">
-        <f t="shared" si="2"/>
-        <v>0.99944895359999997</v>
-      </c>
-      <c r="R15" s="10">
-        <f t="shared" si="6"/>
-        <v>0.99944895359999997</v>
-      </c>
-      <c r="S15" s="10">
-        <f t="shared" si="3"/>
-        <v>3.5152960000000002E-3</v>
-      </c>
-      <c r="T15" s="10">
-        <f t="shared" si="7"/>
         <v>3.5152960000000002E-3</v>
       </c>
       <c r="U15" s="9">
@@ -5271,15 +5206,15 @@
         <v>-I</v>
       </c>
       <c r="X15" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y15" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5307,35 +5242,35 @@
       <c r="J16" s="10"/>
       <c r="K16" s="26"/>
       <c r="L16" s="31">
+        <f>IF($Z16=TRUE,0,IF($Y16=TRUE,0,IF($I16="Ja",IF(ISNUMBER(J16),J16,"-"),IF(ISNUMBER(G16),G16,"-"))))</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="10">
+        <f>IF($Z16=TRUE,0,IF($Y16=TRUE,0,IF($I16="Ja",IF(ISNUMBER(K16),K16,"-"),IF(ISNUMBER(H16),H16,"-"))))</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>NR</v>
+      </c>
+      <c r="Q16" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R16" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="32" t="str">
+        <v>1</v>
+      </c>
+      <c r="S16" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="10">
         <f t="shared" si="5"/>
-        <v>NR</v>
-      </c>
-      <c r="Q16" s="31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="R16" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S16" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="10">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U16" s="9">
@@ -5351,15 +5286,15 @@
         <v>+III</v>
       </c>
       <c r="X16" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y16" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -5396,36 +5331,36 @@
         <v>2.3200000000000005E-5</v>
       </c>
       <c r="L17" s="31">
+        <f>IF($Z17=TRUE,0,IF($Y17=TRUE,0,IF($I17="Ja",IF(ISNUMBER(J17),J17,"-"),IF(ISNUMBER(G17),G17,"-"))))</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M17" s="10">
+        <f>IF($Z17=TRUE,0,IF($Y17=TRUE,0,IF($I17="Ja",IF(ISNUMBER(K17),K17,"-"),IF(ISNUMBER(H17),H17,"-"))))</f>
+        <v>2.3200000000000005E-5</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="0"/>
+        <v>2.3200000000000003</v>
+      </c>
+      <c r="O17" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>-I</v>
+      </c>
+      <c r="Q17" s="31">
+        <f t="shared" si="1"/>
+        <v>0.9999768</v>
+      </c>
+      <c r="R17" s="10">
         <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
-      <c r="M17" s="10">
-        <f t="shared" si="0"/>
-        <v>2.3200000000000005E-5</v>
-      </c>
-      <c r="N17" s="11">
-        <f t="shared" si="1"/>
-        <v>2.3200000000000003E-4</v>
-      </c>
-      <c r="O17" s="32" t="str">
+        <v>0.9999768</v>
+      </c>
+      <c r="S17" s="10">
+        <f t="shared" si="2"/>
+        <v>1.4800000000000002E-4</v>
+      </c>
+      <c r="T17" s="10">
         <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="Q17" s="31">
-        <f t="shared" si="2"/>
-        <v>0.9999768</v>
-      </c>
-      <c r="R17" s="10">
-        <f t="shared" si="6"/>
-        <v>0.9999768</v>
-      </c>
-      <c r="S17" s="10">
-        <f t="shared" si="3"/>
-        <v>1.4800000000000002</v>
-      </c>
-      <c r="T17" s="10">
-        <f t="shared" si="7"/>
-        <v>1.4800000000000002</v>
+        <v>1.4800000000000002E-4</v>
       </c>
       <c r="U17" s="9">
         <f t="array" ref="U17">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M17,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -5440,15 +5375,15 @@
         <v>-I</v>
       </c>
       <c r="X17" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y17" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z17" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5472,7 +5407,7 @@
         <v>2.3800000000000001E-4</v>
       </c>
       <c r="H18" s="26">
-        <f t="shared" ref="H18:H22" si="11">G18*2.32</f>
+        <f t="shared" ref="H18:H22" si="9">G18*2.32</f>
         <v>5.5216E-4</v>
       </c>
       <c r="I18" s="8" t="s">
@@ -5485,36 +5420,36 @@
         <v>2.3200000000000003E-10</v>
       </c>
       <c r="L18" s="31">
+        <f>IF($Z18=TRUE,0,IF($Y18=TRUE,0,IF($I18="Ja",IF(ISNUMBER(J18),J18,"-"),IF(ISNUMBER(G18),G18,"-"))))</f>
+        <v>1E-10</v>
+      </c>
+      <c r="M18" s="10">
+        <f>IF($Z18=TRUE,0,IF($Y18=TRUE,0,IF($I18="Ja",IF(ISNUMBER(K18),K18,"-"),IF(ISNUMBER(H18),H18,"-"))))</f>
+        <v>2.3200000000000003E-10</v>
+      </c>
+      <c r="N18" s="11">
+        <f t="shared" si="0"/>
+        <v>2.3200000000000003</v>
+      </c>
+      <c r="O18" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>-I</v>
+      </c>
+      <c r="Q18" s="31">
+        <f t="shared" si="1"/>
+        <v>0.99999999976800003</v>
+      </c>
+      <c r="R18" s="10">
         <f t="shared" si="4"/>
-        <v>2.3800000000000001E-4</v>
-      </c>
-      <c r="M18" s="10">
-        <f t="shared" si="0"/>
-        <v>2.3200000000000003E-10</v>
-      </c>
-      <c r="N18" s="11">
-        <f t="shared" si="1"/>
-        <v>9.7478991596638658E-7</v>
-      </c>
-      <c r="O18" s="32" t="str">
+        <v>0.99999999976800003</v>
+      </c>
+      <c r="S18" s="10">
+        <f t="shared" si="2"/>
+        <v>1.4800000000000001E-9</v>
+      </c>
+      <c r="T18" s="10">
         <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="Q18" s="31">
-        <f t="shared" si="2"/>
-        <v>0.99999999976800003</v>
-      </c>
-      <c r="R18" s="10">
-        <f t="shared" si="6"/>
-        <v>0.99999999976800003</v>
-      </c>
-      <c r="S18" s="10">
-        <f t="shared" si="3"/>
-        <v>3.5224000000000002E-3</v>
-      </c>
-      <c r="T18" s="10">
-        <f t="shared" si="7"/>
-        <v>3.5224000000000002E-3</v>
+        <v>1.4800000000000001E-9</v>
       </c>
       <c r="U18" s="9">
         <f t="array" ref="U18">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M18,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -5529,15 +5464,15 @@
         <v>-I</v>
       </c>
       <c r="X18" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y18" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z18" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5569,35 +5504,35 @@
       <c r="J19" s="10"/>
       <c r="K19" s="26"/>
       <c r="L19" s="31" t="str">
-        <f t="shared" si="4"/>
+        <f>IF($Z19=TRUE,0,IF($Y19=TRUE,0,IF($I19="Ja",IF(ISNUMBER(J19),J19,"-"),IF(ISNUMBER(G19),G19,"-"))))</f>
         <v>-</v>
       </c>
       <c r="M19" s="10" t="str">
+        <f>IF($Z19=TRUE,0,IF($Y19=TRUE,0,IF($I19="Ja",IF(ISNUMBER(K19),K19,"-"),IF(ISNUMBER(H19),H19,"-"))))</f>
+        <v>-</v>
+      </c>
+      <c r="N19" s="11" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="N19" s="11" t="str">
+      <c r="O19" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="Q19" s="31" t="e">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="O19" s="32" t="str">
-        <f t="shared" si="5"/>
-        <v>D</v>
-      </c>
-      <c r="Q19" s="31" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R19" s="10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S19" s="10" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="R19" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S19" s="10" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="T19" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U19" s="9">
@@ -5613,15 +5548,15 @@
         <v>+III</v>
       </c>
       <c r="X19" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Y19" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Y19" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z19" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5657,36 +5592,36 @@
         <v>0</v>
       </c>
       <c r="L20" s="31">
+        <f>IF($Z20=TRUE,0,IF($Y20=TRUE,0,IF($I20="Ja",IF(ISNUMBER(J20),J20,"-"),IF(ISNUMBER(G20),G20,"-"))))</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="10">
+        <f>IF($Z20=TRUE,0,IF($Y20=TRUE,0,IF($I20="Ja",IF(ISNUMBER(K20),K20,"-"),IF(ISNUMBER(H20),H20,"-"))))</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>+III</v>
+      </c>
+      <c r="Q20" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R20" s="10">
         <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="M20" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="32" t="str">
+        <v>1</v>
+      </c>
+      <c r="S20" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="10">
         <f t="shared" si="5"/>
-        <v>+III</v>
-      </c>
-      <c r="Q20" s="31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="R20" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="S20" s="10">
-        <f t="shared" si="3"/>
-        <v>7.4</v>
-      </c>
-      <c r="T20" s="10">
-        <f t="shared" si="7"/>
-        <v>7.4</v>
+        <v>0</v>
       </c>
       <c r="U20" s="9">
         <f t="array" ref="U20">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M20,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -5705,11 +5640,11 @@
         <v>0</v>
       </c>
       <c r="Y20" s="9" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z20" s="12" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5733,7 +5668,7 @@
         <v>0.1</v>
       </c>
       <c r="H21" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0.23199999999999998</v>
       </c>
       <c r="I21" s="8" t="s">
@@ -5746,36 +5681,36 @@
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="L21" s="31">
+        <f>IF($Z21=TRUE,0,IF($Y21=TRUE,0,IF($I21="Ja",IF(ISNUMBER(J21),J21,"-"),IF(ISNUMBER(G21),G21,"-"))))</f>
+        <v>1E-8</v>
+      </c>
+      <c r="M21" s="10">
+        <f>IF($Z21=TRUE,0,IF($Y21=TRUE,0,IF($I21="Ja",IF(ISNUMBER(K21),K21,"-"),IF(ISNUMBER(H21),H21,"-"))))</f>
+        <v>2.3200000000000003E-8</v>
+      </c>
+      <c r="N21" s="11">
+        <f t="shared" si="0"/>
+        <v>2.3200000000000003</v>
+      </c>
+      <c r="O21" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>-I</v>
+      </c>
+      <c r="Q21" s="31">
+        <f t="shared" si="1"/>
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="R21" s="10">
         <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
-      <c r="M21" s="10">
-        <f t="shared" si="0"/>
-        <v>2.3200000000000003E-8</v>
-      </c>
-      <c r="N21" s="11">
-        <f t="shared" si="1"/>
-        <v>2.3200000000000001E-7</v>
-      </c>
-      <c r="O21" s="32" t="str">
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="S21" s="10">
+        <f t="shared" si="2"/>
+        <v>1.48E-7</v>
+      </c>
+      <c r="T21" s="10">
         <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="Q21" s="31">
-        <f t="shared" si="2"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="R21" s="10">
-        <f t="shared" si="6"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="S21" s="10">
-        <f t="shared" si="3"/>
-        <v>1.4800000000000002</v>
-      </c>
-      <c r="T21" s="10">
-        <f t="shared" si="7"/>
-        <v>1.4800000000000002</v>
+        <v>1.48E-7</v>
       </c>
       <c r="U21" s="9">
         <f t="array" ref="U21">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M21,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -5790,15 +5725,15 @@
         <v>-I</v>
       </c>
       <c r="X21" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y21" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z21" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5822,7 +5757,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="H22" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0.22968</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -5835,36 +5770,36 @@
         <v>2.3200000000000003E-8</v>
       </c>
       <c r="L22" s="31">
+        <f>IF($Z22=TRUE,0,IF($Y22=TRUE,0,IF($I22="Ja",IF(ISNUMBER(J22),J22,"-"),IF(ISNUMBER(G22),G22,"-"))))</f>
+        <v>1E-8</v>
+      </c>
+      <c r="M22" s="10">
+        <f>IF($Z22=TRUE,0,IF($Y22=TRUE,0,IF($I22="Ja",IF(ISNUMBER(K22),K22,"-"),IF(ISNUMBER(H22),H22,"-"))))</f>
+        <v>2.3200000000000003E-8</v>
+      </c>
+      <c r="N22" s="11">
+        <f t="shared" si="0"/>
+        <v>2.3200000000000003</v>
+      </c>
+      <c r="O22" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>-I</v>
+      </c>
+      <c r="Q22" s="31">
+        <f t="shared" si="1"/>
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="R22" s="10">
         <f t="shared" si="4"/>
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="M22" s="10">
-        <f>IF($Z22=TRUE,0,IF($Y22=TRUE,0,IF(I22="Ja",IF(ISNUMBER(K22),K22,"-"),IF(ISNUMBER(H22),H22,"-"))))</f>
-        <v>2.3200000000000003E-8</v>
-      </c>
-      <c r="N22" s="11">
-        <f t="shared" si="1"/>
-        <v>2.3434343434343436E-7</v>
-      </c>
-      <c r="O22" s="32" t="str">
+        <v>0.99999997679999997</v>
+      </c>
+      <c r="S22" s="10">
+        <f t="shared" si="2"/>
+        <v>1.48E-7</v>
+      </c>
+      <c r="T22" s="10">
         <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="Q22" s="31">
-        <f t="shared" si="2"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="R22" s="10">
-        <f t="shared" si="6"/>
-        <v>0.99999997679999997</v>
-      </c>
-      <c r="S22" s="10">
-        <f t="shared" si="3"/>
-        <v>1.4652000000000001</v>
-      </c>
-      <c r="T22" s="10">
-        <f t="shared" si="7"/>
-        <v>1.4652000000000001</v>
+        <v>1.48E-7</v>
       </c>
       <c r="U22" s="9">
         <f t="array" ref="U22">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M22,'Normen en duidingsklassen'!$E$13:$E$20))</f>
@@ -5879,15 +5814,15 @@
         <v>-I</v>
       </c>
       <c r="X22" s="9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="9" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="12" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y22" s="9" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z22" s="12" t="b">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -6107,23 +6042,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11:H30">
-    <cfRule type="expression" dxfId="79" priority="11">
+    <cfRule type="expression" dxfId="70" priority="11">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:K30">
-    <cfRule type="expression" dxfId="78" priority="10">
+    <cfRule type="expression" dxfId="69" priority="10">
       <formula>IF($I11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11:O30">
-    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6672,23 +6607,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11:G16">
-    <cfRule type="expression" dxfId="68" priority="11">
+    <cfRule type="expression" dxfId="59" priority="11">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I16">
-    <cfRule type="expression" dxfId="67" priority="10">
+    <cfRule type="expression" dxfId="58" priority="10">
       <formula>IF($H11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K16">
-    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7200,23 +7135,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="57" priority="11">
+    <cfRule type="expression" dxfId="48" priority="11">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="56" priority="10">
+    <cfRule type="expression" dxfId="47" priority="10">
       <formula>IF($H11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7321,7 +7256,7 @@
   <dimension ref="B2:V30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:K11"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7479,23 +7414,23 @@
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="5">
-        <f>IF($V11=TRUE,0,IF($U11=TRUE,0,IF(H11="Ja",IF(ISNUMBER(I11),I11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
+        <f t="shared" ref="J11:J22" si="0">IF($V11=TRUE,0,IF($U11=TRUE,0,IF(H11="Ja",IF(ISNUMBER(I11),I11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
         <v>0</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f>IF($V11=TRUE,"NR",IF($U11=TRUE,"ND",IF($T11=TRUE,"D",S11)))</f>
+        <f t="shared" ref="K11:K22" si="1">IF($V11=TRUE,"NR",IF($U11=TRUE,"ND",IF($T11=TRUE,"D",S11)))</f>
         <v>ND</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11:M12" si="0">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11:M12" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N12" si="1">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11:N12" si="3">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11:O12" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11:O12" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -7553,27 +7488,27 @@
         <v>0</v>
       </c>
       <c r="J12" s="10">
-        <f>IF($V12=TRUE,0,IF($U12=TRUE,0,IF(H12="Ja",IF(ISNUMBER(I12),I12,"-"),IF(ISNUMBER(G12),G12,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12" s="32" t="str">
-        <f>IF($V12=TRUE,"NR",IF($U12=TRUE,"ND",IF($T12=TRUE,"D",S12)))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M12" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N12" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P13" si="3">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P13" si="5">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -7589,15 +7524,15 @@
         <v>+III</v>
       </c>
       <c r="T12" s="9" t="b">
-        <f t="shared" ref="T12:T22" si="4">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="6">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
       <c r="U12" s="9" t="b">
-        <f t="shared" ref="U12:U22" si="5">IF($E12="Ja",IF($H12="Nee",NOT(ISNUMBER($G12)),FALSE),FALSE)</f>
+        <f t="shared" ref="U12:U22" si="7">IF($E12="Ja",IF($H12="Nee",NOT(ISNUMBER($G12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
       <c r="V12" s="12" t="b">
-        <f t="shared" ref="V12:V22" si="6">IF(E12="Nee",TRUE,FALSE)</f>
+        <f t="shared" ref="V12:V22" si="8">IF(E12="Nee",TRUE,FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -7627,27 +7562,27 @@
         <v>5.9999999999999997E-7</v>
       </c>
       <c r="J13" s="10">
-        <f>IF($V13=TRUE,0,IF($U13=TRUE,0,IF(H13="Ja",IF(ISNUMBER(I13),I13,"-"),IF(ISNUMBER(G13),G13,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>5.9999999999999997E-7</v>
       </c>
       <c r="K13" s="32" t="str">
-        <f>IF($V13=TRUE,"NR",IF($U13=TRUE,"ND",IF($T13=TRUE,"D",S13)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" ref="M13:M22" si="7">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
+        <f t="shared" ref="M13:M22" si="9">IF(AND(F13="Geen faalkans",H13="Nee"),1,1-J13)</f>
         <v>0.99999939999999998</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" ref="N13:N22" si="8">IF(J13="-",1,M13)</f>
+        <f t="shared" ref="N13:N22" si="10">IF(J13="-",1,M13)</f>
         <v>0.99999939999999998</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" ref="O13:O22" si="9">IF(AND(F13="Geen faalkans",H13="Nee"),0,J13*$C$3)</f>
+        <f t="shared" ref="O13:O22" si="11">IF(AND(F13="Geen faalkans",H13="Nee"),0,J13*$C$3)</f>
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="Q13" s="9">
@@ -7663,15 +7598,15 @@
         <v>-I</v>
       </c>
       <c r="T13" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U13" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V13" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -7699,27 +7634,27 @@
       </c>
       <c r="I14" s="26"/>
       <c r="J14" s="10">
-        <f>IF($V14=TRUE,0,IF($U14=TRUE,0,IF(H14="Ja",IF(ISNUMBER(I14),I14,"-"),IF(ISNUMBER(G14),G14,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="K14" s="32" t="str">
-        <f>IF($V14=TRUE,"NR",IF($U14=TRUE,"ND",IF($T14=TRUE,"D",S14)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M14" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.99999499999999997</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99999499999999997</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" ref="P14:P22" si="10">IF(J14="-",0,O14)</f>
+        <f t="shared" ref="P14:P22" si="12">IF(J14="-",0,O14)</f>
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="Q14" s="9">
@@ -7735,15 +7670,15 @@
         <v>-I</v>
       </c>
       <c r="T14" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U14" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V14" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -7773,27 +7708,27 @@
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="J15" s="10">
-        <f>IF($V15=TRUE,0,IF($U15=TRUE,0,IF(H15="Ja",IF(ISNUMBER(I15),I15,"-"),IF(ISNUMBER(G15),G15,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="K15" s="32" t="str">
-        <f>IF($V15=TRUE,"NR",IF($U15=TRUE,"ND",IF($T15=TRUE,"D",S15)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M15" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.999999992</v>
       </c>
       <c r="N15" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.999999992</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.4000000000000003E-8</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.4000000000000003E-8</v>
       </c>
       <c r="Q15" s="9">
@@ -7809,15 +7744,15 @@
         <v>-I</v>
       </c>
       <c r="T15" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U15" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V15" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -7847,27 +7782,27 @@
         <v>0</v>
       </c>
       <c r="J16" s="10">
-        <f>IF($V16=TRUE,0,IF($U16=TRUE,0,IF(H16="Ja",IF(ISNUMBER(I16),I16,"-"),IF(ISNUMBER(G16),G16,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K16" s="32" t="str">
-        <f>IF($V16=TRUE,"NR",IF($U16=TRUE,"ND",IF($T16=TRUE,"D",S16)))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M16" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
@@ -7883,15 +7818,15 @@
         <v>+III</v>
       </c>
       <c r="T16" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U16" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V16" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -7921,27 +7856,27 @@
         <v>2.546E-5</v>
       </c>
       <c r="J17" s="10">
-        <f>IF($V17=TRUE,0,IF($U17=TRUE,0,IF(H17="Ja",IF(ISNUMBER(I17),I17,"-"),IF(ISNUMBER(G17),G17,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>2.546E-5</v>
       </c>
       <c r="K17" s="32" t="str">
-        <f>IF($V17=TRUE,"NR",IF($U17=TRUE,"ND",IF($T17=TRUE,"D",S17)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M17" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.99997453999999997</v>
       </c>
       <c r="N17" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99997453999999997</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>7.6379999999999997E-5</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>7.6379999999999997E-5</v>
       </c>
       <c r="Q17" s="9">
@@ -7957,15 +7892,15 @@
         <v>-I</v>
       </c>
       <c r="T17" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U17" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V17" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -7993,27 +7928,27 @@
       </c>
       <c r="I18" s="26"/>
       <c r="J18" s="10">
-        <f>IF($V18=TRUE,0,IF($U18=TRUE,0,IF(H18="Ja",IF(ISNUMBER(I18),I18,"-"),IF(ISNUMBER(G18),G18,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>6.6600000000000003E-4</v>
       </c>
       <c r="K18" s="32" t="str">
-        <f>IF($V18=TRUE,"NR",IF($U18=TRUE,"ND",IF($T18=TRUE,"D",S18)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M18" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.99933399999999994</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99933399999999994</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.9980000000000002E-3</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9980000000000002E-3</v>
       </c>
       <c r="Q18" s="9">
@@ -8029,15 +7964,15 @@
         <v>-I</v>
       </c>
       <c r="T18" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U18" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V18" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -8067,27 +8002,27 @@
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="J19" s="10">
-        <f>IF($V19=TRUE,0,IF($U19=TRUE,0,IF(H19="Ja",IF(ISNUMBER(I19),I19,"-"),IF(ISNUMBER(G19),G19,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="K19" s="32" t="str">
-        <f>IF($V19=TRUE,"NR",IF($U19=TRUE,"ND",IF($T19=TRUE,"D",S19)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M19" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.99870000000000003</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99870000000000003</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="Q19" s="9">
@@ -8103,15 +8038,15 @@
         <v>-I</v>
       </c>
       <c r="T19" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U19" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V19" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -8139,27 +8074,27 @@
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="10">
-        <f>IF($V20=TRUE,0,IF($U20=TRUE,0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K20" s="32" t="str">
-        <f>IF($V20=TRUE,"NR",IF($U20=TRUE,"ND",IF($T20=TRUE,"D",S20)))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q20" s="9">
@@ -8175,15 +8110,15 @@
         <v>+III</v>
       </c>
       <c r="T20" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U20" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V20" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -8213,27 +8148,27 @@
         <v>0</v>
       </c>
       <c r="J21" s="10">
-        <f>IF($V21=TRUE,0,IF($U21=TRUE,0,IF(H21="Ja",IF(ISNUMBER(I21),I21,"-"),IF(ISNUMBER(G21),G21,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K21" s="32" t="str">
-        <f>IF($V21=TRUE,"NR",IF($U21=TRUE,"ND",IF($T21=TRUE,"D",S21)))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M21" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q21" s="9">
@@ -8249,15 +8184,15 @@
         <v>+III</v>
       </c>
       <c r="T21" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U21" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V21" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -8283,27 +8218,27 @@
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="10">
-        <f>IF($V22=TRUE,0,IF($U22=TRUE,0,IF(H22="Ja",IF(ISNUMBER(I22),I22,"-"),IF(ISNUMBER(G22),G22,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K22" s="32" t="str">
-        <f>IF($V22=TRUE,"NR",IF($U22=TRUE,"ND",IF($T22=TRUE,"D",S22)))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M22" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q22" s="9">
@@ -8319,15 +8254,15 @@
         <v>+III</v>
       </c>
       <c r="T22" s="9" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U22" s="9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V22" s="12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -8471,23 +8406,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11:G28">
-    <cfRule type="expression" dxfId="46" priority="5">
+    <cfRule type="expression" dxfId="37" priority="5">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I28">
-    <cfRule type="expression" dxfId="45" priority="4">
+    <cfRule type="expression" dxfId="36" priority="4">
       <formula>IF($H11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K28">
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8744,23 +8679,23 @@
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="5">
-        <f>IF($V11=TRUE,0,IF($U11=TRUE,0,IF(H11="Ja",IF(ISNUMBER(I11),I11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
+        <f t="shared" ref="J11:J22" si="0">IF($V11=TRUE,0,IF($U11=TRUE,0,IF(H11="Ja",IF(ISNUMBER(I11),I11,"-"),IF(ISNUMBER(G11),G11,"-"))))</f>
         <v>0</v>
       </c>
       <c r="K11" s="30" t="str">
-        <f>IF($V11=TRUE,"NR",IF($U11=TRUE,"ND",IF($T11=TRUE,"D",S11)))</f>
+        <f t="shared" ref="K11:K22" si="1">IF($V11=TRUE,"NR",IF($U11=TRUE,"ND",IF($T11=TRUE,"D",S11)))</f>
         <v>NR</v>
       </c>
       <c r="M11" s="31">
-        <f t="shared" ref="M11" si="0">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
+        <f t="shared" ref="M11" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),1,1-J11)</f>
         <v>1</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11" si="1">IF(J11="-",1,M11)</f>
+        <f t="shared" ref="N11" si="3">IF(J11="-",1,M11)</f>
         <v>1</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11" si="2">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
+        <f t="shared" ref="O11" si="4">IF(AND(F11="Geen faalkans",H11="Nee"),0,J11*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P11" s="10">
@@ -8814,27 +8749,27 @@
       </c>
       <c r="I12" s="26"/>
       <c r="J12" s="10">
-        <f>IF($V12=TRUE,0,IF($U12=TRUE,0,IF(H12="Ja",IF(ISNUMBER(I12),I12,"-"),IF(ISNUMBER(G12),G12,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12" s="32" t="str">
-        <f>IF($V12=TRUE,"NR",IF($U12=TRUE,"ND",IF($T12=TRUE,"D",S12)))</f>
+        <f t="shared" si="1"/>
         <v>ND</v>
       </c>
       <c r="M12" s="31">
-        <f t="shared" ref="M12:M22" si="3">IF(AND(F12="Geen faalkans",H12="Nee"),1,1-J12)</f>
+        <f t="shared" ref="M12:M22" si="5">IF(AND(F12="Geen faalkans",H12="Nee"),1,1-J12)</f>
         <v>1</v>
       </c>
       <c r="N12" s="10">
-        <f t="shared" ref="N12:N22" si="4">IF(J12="-",1,M12)</f>
+        <f t="shared" ref="N12:N22" si="6">IF(J12="-",1,M12)</f>
         <v>1</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" ref="O12:O22" si="5">IF(AND(F12="Geen faalkans",H12="Nee"),0,J12*$C$3)</f>
+        <f t="shared" ref="O12:O22" si="7">IF(AND(F12="Geen faalkans",H12="Nee"),0,J12*$C$3)</f>
         <v>0</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P22" si="6">IF(J12="-",0,O12)</f>
+        <f t="shared" ref="P12:P22" si="8">IF(J12="-",0,O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="9">
@@ -8850,15 +8785,15 @@
         <v>+III</v>
       </c>
       <c r="T12" s="9" t="b">
-        <f t="shared" ref="T12:T22" si="7">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
+        <f t="shared" ref="T12:T22" si="9">IF($E12="Ja",IF($H12="Ja",NOT(ISNUMBER($I12)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
       <c r="U12" s="9" t="b">
-        <f t="shared" ref="U12:U22" si="8">IF($E12="Ja",IF($H12="Nee",NOT(ISNUMBER($G12)),FALSE),FALSE)</f>
+        <f t="shared" ref="U12:U22" si="10">IF($E12="Ja",IF($H12="Nee",NOT(ISNUMBER($G12)),FALSE),FALSE)</f>
         <v>1</v>
       </c>
       <c r="V12" s="12" t="b">
-        <f t="shared" ref="V12:V22" si="9">IF(E12="Nee",TRUE,FALSE)</f>
+        <f t="shared" ref="V12:V22" si="11">IF(E12="Nee",TRUE,FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -8888,27 +8823,27 @@
         <v>0</v>
       </c>
       <c r="J13" s="10">
-        <f>IF($V13=TRUE,0,IF($U13=TRUE,0,IF(H13="Ja",IF(ISNUMBER(I13),I13,"-"),IF(ISNUMBER(G13),G13,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K13" s="32" t="str">
-        <f>IF($V13=TRUE,"NR",IF($U13=TRUE,"ND",IF($T13=TRUE,"D",S13)))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M13" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q13" s="9">
@@ -8924,15 +8859,15 @@
         <v>+III</v>
       </c>
       <c r="T13" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U13" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V13" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -8960,27 +8895,27 @@
       </c>
       <c r="I14" s="26"/>
       <c r="J14" s="10">
-        <f>IF($V14=TRUE,0,IF($U14=TRUE,0,IF(H14="Ja",IF(ISNUMBER(I14),I14,"-"),IF(ISNUMBER(G14),G14,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="K14" s="32" t="str">
-        <f>IF($V14=TRUE,"NR",IF($U14=TRUE,"ND",IF($T14=TRUE,"D",S14)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M14" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.99977199999999999</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99977199999999999</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.2800000000000001E-4</v>
       </c>
       <c r="Q14" s="9">
@@ -8996,15 +8931,15 @@
         <v>-I</v>
       </c>
       <c r="T14" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U14" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V14" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9034,27 +8969,27 @@
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="J15" s="10">
-        <f>IF($V15=TRUE,0,IF($U15=TRUE,0,IF(H15="Ja",IF(ISNUMBER(I15),I15,"-"),IF(ISNUMBER(G15),G15,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="K15" s="32" t="str">
-        <f>IF($V15=TRUE,"NR",IF($U15=TRUE,"ND",IF($T15=TRUE,"D",S15)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M15" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.99673</v>
       </c>
       <c r="N15" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99673</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.2699999999999999E-3</v>
       </c>
       <c r="Q15" s="9">
@@ -9070,15 +9005,15 @@
         <v>-I</v>
       </c>
       <c r="T15" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U15" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V15" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9104,27 +9039,27 @@
       </c>
       <c r="I16" s="26"/>
       <c r="J16" s="10">
-        <f>IF($V16=TRUE,0,IF($U16=TRUE,0,IF(H16="Ja",IF(ISNUMBER(I16),I16,"-"),IF(ISNUMBER(G16),G16,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K16" s="32" t="str">
-        <f>IF($V16=TRUE,"NR",IF($U16=TRUE,"ND",IF($T16=TRUE,"D",S16)))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M16" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
@@ -9140,15 +9075,15 @@
         <v>+III</v>
       </c>
       <c r="T16" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U16" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V16" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -9174,27 +9109,27 @@
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="10">
-        <f>IF($V17=TRUE,0,IF($U17=TRUE,0,IF(H17="Ja",IF(ISNUMBER(I17),I17,"-"),IF(ISNUMBER(G17),G17,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K17" s="32" t="str">
-        <f>IF($V17=TRUE,"NR",IF($U17=TRUE,"ND",IF($T17=TRUE,"D",S17)))</f>
+        <f t="shared" si="1"/>
         <v>NR</v>
       </c>
       <c r="M17" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N17" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q17" s="9">
@@ -9210,15 +9145,15 @@
         <v>+III</v>
       </c>
       <c r="T17" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U17" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V17" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -9246,27 +9181,27 @@
       </c>
       <c r="I18" s="26"/>
       <c r="J18" s="10">
-        <f>IF($V18=TRUE,0,IF($U18=TRUE,0,IF(H18="Ja",IF(ISNUMBER(I18),I18,"-"),IF(ISNUMBER(G18),G18,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K18" s="32" t="str">
-        <f>IF($V18=TRUE,"NR",IF($U18=TRUE,"ND",IF($T18=TRUE,"D",S18)))</f>
+        <f t="shared" si="1"/>
         <v>+III</v>
       </c>
       <c r="M18" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q18" s="9">
@@ -9282,15 +9217,15 @@
         <v>+III</v>
       </c>
       <c r="T18" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U18" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V18" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9318,27 +9253,27 @@
       </c>
       <c r="I19" s="26"/>
       <c r="J19" s="10" t="str">
-        <f>IF($V19=TRUE,0,IF($U19=TRUE,0,IF(H19="Ja",IF(ISNUMBER(I19),I19,"-"),IF(ISNUMBER(G19),G19,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="K19" s="32" t="str">
-        <f>IF($V19=TRUE,"NR",IF($U19=TRUE,"ND",IF($T19=TRUE,"D",S19)))</f>
+        <f t="shared" si="1"/>
         <v>D</v>
       </c>
       <c r="M19" s="31" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N19" s="10">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="O19" s="10" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="N19" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="10" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="P19" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q19" s="9">
@@ -9354,15 +9289,15 @@
         <v>+III</v>
       </c>
       <c r="T19" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="U19" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V19" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9390,27 +9325,27 @@
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="10">
-        <f>IF($V20=TRUE,0,IF($U20=TRUE,0,IF(H20="Ja",IF(ISNUMBER(I20),I20,"-"),IF(ISNUMBER(G20),G20,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="K20" s="32" t="str">
-        <f>IF($V20=TRUE,"NR",IF($U20=TRUE,"ND",IF($T20=TRUE,"D",S20)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.99999800000000005</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99999800000000005</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="Q20" s="9">
@@ -9426,15 +9361,15 @@
         <v>-I</v>
       </c>
       <c r="T20" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U20" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V20" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9464,27 +9399,27 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="J21" s="10">
-        <f>IF($V21=TRUE,0,IF($U21=TRUE,0,IF(H21="Ja",IF(ISNUMBER(I21),I21,"-"),IF(ISNUMBER(G21),G21,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K21" s="32" t="str">
-        <f>IF($V21=TRUE,"NR",IF($U21=TRUE,"ND",IF($T21=TRUE,"D",S21)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M21" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.99950000000000006</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99950000000000006</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q21" s="9">
@@ -9500,15 +9435,15 @@
         <v>-I</v>
       </c>
       <c r="T21" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U21" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V21" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9536,27 +9471,27 @@
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="10">
-        <f>IF($V22=TRUE,0,IF($U22=TRUE,0,IF(H22="Ja",IF(ISNUMBER(I22),I22,"-"),IF(ISNUMBER(G22),G22,"-"))))</f>
+        <f t="shared" si="0"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="K22" s="32" t="str">
-        <f>IF($V22=TRUE,"NR",IF($U22=TRUE,"ND",IF($T22=TRUE,"D",S22)))</f>
+        <f t="shared" si="1"/>
         <v>-I</v>
       </c>
       <c r="M22" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.99999999799999995</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99999999799999995</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="Q22" s="9">
@@ -9572,15 +9507,15 @@
         <v>-I</v>
       </c>
       <c r="T22" s="9" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U22" s="9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V22" s="12" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9724,23 +9659,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11:G28">
-    <cfRule type="expression" dxfId="35" priority="5">
+    <cfRule type="expression" dxfId="26" priority="5">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I28">
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>IF($H11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K28">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10962,23 +10897,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G11:G15 G17:G27">
-    <cfRule type="expression" dxfId="24" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I27">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>IF($H11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K27">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>